<commit_message>
New BDD estimation for presum data
</commit_message>
<xml_diff>
--- a/explore/pseudoboolean/mcb-scaling.xlsx
+++ b/explore/pseudoboolean/mcb-scaling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryant/repos/pgbdd/explore/pseudoboolean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D52AA79-4E02-FC44-B4D8-FB587F6707D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C9FCD5-168D-C041-8F50-AC8109AFD251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9900" yWindow="11300" windowWidth="32440" windowHeight="15860" firstSheet="1" activeTab="5" xr2:uid="{544DE29A-88F0-0E4C-87E1-E71170600DAE}"/>
   </bookViews>
@@ -3453,91 +3453,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>10452</c:v>
+                  <c:v>13488</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19008</c:v>
+                  <c:v>24624</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30168</c:v>
+                  <c:v>39168</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44832</c:v>
+                  <c:v>58320</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>61956</c:v>
+                  <c:v>80688</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>107724</c:v>
+                  <c:v>140592</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>166068</c:v>
+                  <c:v>217008</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>240876</c:v>
+                  <c:v>315120</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>327396</c:v>
+                  <c:v>428592</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>554868</c:v>
+                  <c:v>727344</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>842436</c:v>
+                  <c:v>1105200</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1203636</c:v>
+                  <c:v>1580208</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1620900</c:v>
+                  <c:v>2128944</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2703684</c:v>
+                  <c:v>3554352</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4064868</c:v>
+                  <c:v>5346864</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5754564</c:v>
+                  <c:v>7573296</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7705380</c:v>
+                  <c:v>10143792</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12716388</c:v>
+                  <c:v>16751664</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18990756</c:v>
+                  <c:v>25027632</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>26720868</c:v>
+                  <c:v>35228208</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>35642916</c:v>
+                  <c:v>47001648</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>58378404</c:v>
+                  <c:v>77021232</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>86761764</c:v>
+                  <c:v>114505776</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>121546404</c:v>
+                  <c:v>160459824</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>161688612</c:v>
+                  <c:v>213491760</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>263331108</c:v>
+                  <c:v>347836464</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>389933604</c:v>
+                  <c:v>515199024</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>544477476</c:v>
+                  <c:v>719554608</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>722810916</c:v>
+                  <c:v>955367472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9286,7 +9286,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9327,13 +9327,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="3">
-        <v>10452</v>
+        <v>13488</v>
       </c>
       <c r="C4" s="4">
         <v>5733</v>
       </c>
       <c r="D4" s="4">
-        <f>POWER(A4,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" ref="D4:D20" si="0">POWER(A4,$C$2)*B$2/POWER(A$4,$C$2)</f>
         <v>2000</v>
       </c>
     </row>
@@ -9342,13 +9342,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="3">
-        <v>19008</v>
+        <v>24624</v>
       </c>
       <c r="C5" s="4">
         <v>9591</v>
       </c>
       <c r="D5" s="4">
-        <f>POWER(A5,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>3341.3581249724675</v>
       </c>
     </row>
@@ -9357,13 +9357,13 @@
         <v>12</v>
       </c>
       <c r="B6" s="3">
-        <v>30168</v>
+        <v>39168</v>
       </c>
       <c r="C6" s="4">
         <v>15480</v>
       </c>
       <c r="D6" s="4">
-        <f>POWER(A6,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>5082.0612095558517</v>
       </c>
     </row>
@@ -9372,13 +9372,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="3">
-        <v>44832</v>
+        <v>58320</v>
       </c>
       <c r="C7" s="4">
         <v>23547</v>
       </c>
       <c r="D7" s="4">
-        <f>POWER(A7,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>7244.6516473208876</v>
       </c>
     </row>
@@ -9387,13 +9387,13 @@
         <v>16</v>
       </c>
       <c r="B8" s="3">
-        <v>61956</v>
+        <v>80688</v>
       </c>
       <c r="C8" s="4">
         <v>31005</v>
       </c>
       <c r="D8" s="4">
-        <f>POWER(A8,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>9849.1553067593322</v>
       </c>
     </row>
@@ -9402,13 +9402,13 @@
         <v>20</v>
       </c>
       <c r="B9" s="3">
-        <v>107724</v>
+        <v>140592</v>
       </c>
       <c r="C9" s="4">
         <v>51846</v>
       </c>
       <c r="D9" s="4">
-        <f>POWER(A9,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>16454.777554177981</v>
       </c>
     </row>
@@ -9417,13 +9417,13 @@
         <v>24</v>
       </c>
       <c r="B10" s="3">
-        <v>166068</v>
+        <v>217008</v>
       </c>
       <c r="C10" s="4">
         <v>73353</v>
       </c>
       <c r="D10" s="4">
-        <f>POWER(A10,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>25027.005065686386</v>
       </c>
     </row>
@@ -9432,13 +9432,13 @@
         <v>28</v>
       </c>
       <c r="B11" s="3">
-        <v>240876</v>
+        <v>315120</v>
       </c>
       <c r="C11" s="4">
         <v>106104</v>
       </c>
       <c r="D11" s="4">
-        <f>POWER(A11,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>35676.849608916593</v>
       </c>
     </row>
@@ -9447,13 +9447,13 @@
         <v>32</v>
       </c>
       <c r="B12" s="3">
-        <v>327396</v>
+        <v>428592</v>
       </c>
       <c r="C12" s="4">
         <v>142611</v>
       </c>
       <c r="D12" s="4">
-        <f>POWER(A12,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>48502.930128332759</v>
       </c>
     </row>
@@ -9462,13 +9462,13 @@
         <v>40</v>
       </c>
       <c r="B13" s="3">
-        <v>554868</v>
+        <v>727344</v>
       </c>
       <c r="C13" s="4">
         <v>234402</v>
       </c>
       <c r="D13" s="4">
-        <f>POWER(A13,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>81032.829834638193</v>
       </c>
     </row>
@@ -9477,13 +9477,13 @@
         <v>48</v>
       </c>
       <c r="B14" s="3">
-        <v>842436</v>
+        <v>1105200</v>
       </c>
       <c r="C14" s="4">
         <v>345960</v>
       </c>
       <c r="D14" s="4">
-        <f>POWER(A14,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>123247.42987749887</v>
       </c>
     </row>
@@ -9492,13 +9492,13 @@
         <v>56</v>
       </c>
       <c r="B15" s="3">
-        <v>1203636</v>
+        <v>1580208</v>
       </c>
       <c r="C15" s="4">
         <v>468630</v>
       </c>
       <c r="D15" s="4">
-        <f>POWER(A15,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>175693.41632705793</v>
       </c>
     </row>
@@ -9507,13 +9507,13 @@
         <v>64</v>
       </c>
       <c r="B16" s="3">
-        <v>1620900</v>
+        <v>2128944</v>
       </c>
       <c r="C16" s="4">
         <v>625566</v>
       </c>
       <c r="D16" s="4">
-        <f>POWER(A16,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>238856.44583342245</v>
       </c>
     </row>
@@ -9522,13 +9522,13 @@
         <v>80</v>
       </c>
       <c r="B17" s="3">
-        <v>2703684</v>
+        <v>3554352</v>
       </c>
       <c r="C17" s="4">
         <v>992862</v>
       </c>
       <c r="D17" s="4">
-        <f>POWER(A17,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>399052.46299377602</v>
       </c>
     </row>
@@ -9537,13 +9537,13 @@
         <v>96</v>
       </c>
       <c r="B18" s="3">
-        <v>4064868</v>
+        <v>5346864</v>
       </c>
       <c r="C18" s="4">
         <v>1454067</v>
       </c>
       <c r="D18" s="4">
-        <f>POWER(A18,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>606941.53901120776</v>
       </c>
     </row>
@@ -9552,13 +9552,13 @@
         <v>112</v>
       </c>
       <c r="B19" s="3">
-        <v>5754564</v>
+        <v>7573296</v>
       </c>
       <c r="C19" s="4">
         <v>1994061</v>
       </c>
       <c r="D19" s="4">
-        <f>POWER(A19,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>865215.87189015734</v>
       </c>
     </row>
@@ -9567,13 +9567,13 @@
         <v>128</v>
       </c>
       <c r="B20" s="3">
-        <v>7705380</v>
+        <v>10143792</v>
       </c>
       <c r="C20" s="4">
         <v>2629767</v>
       </c>
       <c r="D20" s="4">
-        <f>POWER(A20,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" si="0"/>
         <v>1176267.1155169639</v>
       </c>
     </row>
@@ -9582,13 +9582,13 @@
         <v>160</v>
       </c>
       <c r="B21" s="3">
-        <v>12716388</v>
+        <v>16751664</v>
       </c>
       <c r="C21" s="4">
         <v>4154493</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" ref="D21:D32" si="0">POWER(A21,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <f t="shared" ref="D21:D32" si="1">POWER(A21,$C$2)*B$2/POWER(A$4,$C$2)</f>
         <v>1965164.841785264</v>
       </c>
     </row>
@@ -9597,13 +9597,13 @@
         <v>192</v>
       </c>
       <c r="B22" s="3">
-        <v>18990756</v>
+        <v>25027632</v>
       </c>
       <c r="C22" s="4">
         <v>6047664</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2988930.7399224541</v>
       </c>
     </row>
@@ -9612,10 +9612,10 @@
         <v>224</v>
       </c>
       <c r="B23" s="3">
-        <v>26720868</v>
+        <v>35228208</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4260822.748059677</v>
       </c>
     </row>
@@ -9624,10 +9624,10 @@
         <v>256</v>
       </c>
       <c r="B24" s="3">
-        <v>35642916</v>
+        <v>47001648</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5792618.7514801938</v>
       </c>
     </row>
@@ -9636,10 +9636,10 @@
         <v>320</v>
       </c>
       <c r="B25" s="3">
-        <v>58378404</v>
+        <v>77021232</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9677606.8650630899</v>
       </c>
     </row>
@@ -9648,10 +9648,10 @@
         <v>384</v>
       </c>
       <c r="B26" s="3">
-        <v>86761764</v>
+        <v>114505776</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14719221.529321682</v>
       </c>
     </row>
@@ -9660,10 +9660,10 @@
         <v>448</v>
       </c>
       <c r="B27" s="3">
-        <v>121546404</v>
+        <v>160459824</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20982752.490106404</v>
       </c>
     </row>
@@ -9672,10 +9672,10 @@
         <v>512</v>
       </c>
       <c r="B28" s="3">
-        <v>161688612</v>
+        <v>213491760</v>
       </c>
       <c r="D28" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28526200.858087406</v>
       </c>
     </row>
@@ -9684,10 +9684,10 @@
         <v>640</v>
       </c>
       <c r="B29" s="3">
-        <v>263331108</v>
+        <v>347836464</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47658126.505883373</v>
       </c>
     </row>
@@ -9696,10 +9696,10 @@
         <v>768</v>
       </c>
       <c r="B30" s="3">
-        <v>389933604</v>
+        <v>515199024</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>72485949.418442354</v>
       </c>
     </row>
@@ -9708,10 +9708,10 @@
         <v>896</v>
       </c>
       <c r="B31" s="3">
-        <v>544477476</v>
+        <v>719554608</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>103331194.01917462</v>
       </c>
     </row>
@@ -9720,10 +9720,10 @@
         <v>1024</v>
       </c>
       <c r="B32" s="3">
-        <v>722810916</v>
+        <v>955367472</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>140479491.28155696</v>
       </c>
     </row>

</xml_diff>